<commit_message>
[IMP] forlife_business_objective_plan: KHAI BÁO HỆ SỐ TÍNH DOANH THU
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_business_objective_plan/static/xlsx/template_import_bo_employee.xlsx
+++ b/addons/custom/forlife_business_objective_plan/static/xlsx/template_import_bo_employee.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t xml:space="preserve">Mã khu vực</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Vị trí công việc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vị trí kiêm nhiệm</t>
   </si>
   <si>
     <t xml:space="preserve">Mục tiêu cá nhân</t>
@@ -220,17 +223,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="16.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,10 +252,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>3004</v>
@@ -261,15 +267,15 @@
         <v>108275</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>10000000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3005</v>
@@ -278,15 +284,15 @@
         <v>108276</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>10000000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3007</v>
@@ -295,9 +301,9 @@
         <v>108277</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>10000000</v>
       </c>
     </row>

</xml_diff>